<commit_message>
something went wrong while load_workbook() the 6.7KB xlsx, issue reported to openpyxl, waiting for reply
</commit_message>
<xml_diff>
--- a/score-sheets/template.xlsx
+++ b/score-sheets/template.xlsx
@@ -84,9 +84,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -100,53 +99,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -160,6 +120,53 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -167,18 +174,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -190,23 +204,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -219,8 +218,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -235,31 +235,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,151 +415,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -426,6 +426,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -489,7 +498,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -498,7 +507,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -517,65 +526,56 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7"/>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6"/>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="5"/>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="7"/>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2"/>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="4"/>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="5"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="4"/>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="5"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2"/>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="8"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">

</xml_diff>

<commit_message>
considering how to get search-score done
</commit_message>
<xml_diff>
--- a/score-sheets/template.xlsx
+++ b/score-sheets/template.xlsx
@@ -64,8 +64,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -91,40 +91,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -146,10 +129,41 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -161,14 +175,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,44 +220,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,37 +241,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -283,139 +415,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -453,17 +453,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -475,6 +464,50 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -493,87 +526,54 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8"/>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6"/>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6"/>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="5"/>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="5"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="4"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="8"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="3"/>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2"/>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -913,9 +913,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.5"/>

</xml_diff>